<commit_message>
Approximated PWM as a function of tick time (power function). Still not straight, but better start for calibration later
</commit_message>
<xml_diff>
--- a/motor analysis.xlsx
+++ b/motor analysis.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t xml:space="preserve"> rticks</t>
+  </si>
+  <si>
+    <t>tick time</t>
+  </si>
+  <si>
+    <t>right tick time</t>
+  </si>
+  <si>
+    <t>ratio</t>
   </si>
 </sst>
 </file>
@@ -81,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,7 +195,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5085957027353697E-2"/>
+                  <c:y val="-8.4068309643112793E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -664,6 +681,954 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>tick times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39223600174978129"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>left tick time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5919728783902012E-2"/>
+                  <c:y val="-9.387977544473608E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Forward!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Forward!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>80768.9375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77235.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55540.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47285.8125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42148.0625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34722.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38767.6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36029.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34862.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35939.1875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34408.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33812.0625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32287.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31100.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31473.4375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29832.125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27391.9375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28302.0625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26248.625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25835.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24737.9375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23201.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22625.5625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22460.875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19954.686567164179</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928.125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053.0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998.4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18668.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17709.808219178081</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19098.830769230768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18679.880597014926</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17931.939393939392</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15197.105263157895</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16984.895522388058</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348.4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15816.888888888889</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14941.8125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>right tick time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.5808617672790896E-2"/>
+                  <c:y val="5.0258821813939925E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Forward!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Forward!$G$2:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>66271.948717948719</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52032.084210526315</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42487.148936170212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36271.591836734697</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30880.530612244896</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29005.118279569891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30441.972602739726</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28850.372093023256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24794.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25069.842696629214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28396.395061728395</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28232.51282051282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27743.23076923077</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29519.771428571428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27265.972602739726</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29192.753623188404</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28077.294117647059</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26970.523076923077</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26251.1884057971</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25073.313432835821</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24678.686567164179</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24357.353846153845</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22498.424242424244</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22277.476923076923</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22115.323076923076</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20257.030303030304</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928.125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053.0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998.4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19252.0625</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20200.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17484.845070422536</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19555.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18492.3125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18046.5625</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17781.0625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348.4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17983.4375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17794</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14711.938461538462</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="365884864"/>
+        <c:axId val="365891584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="365884864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365891584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="365891584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365884864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1276,7 +2241,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1781,7 +2746,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2440,6 +3405,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4504,20 +5509,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4531,6 +6052,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4915,14 +6466,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4941,8 +6493,17 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>536</v>
       </c>
@@ -4970,6 +6531,7 @@
         <f>D2/E2</f>
         <v>0.82051282051282048</v>
       </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -4996,9 +6558,10 @@
         <v>52032.084210526315</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H44" si="2">D3/E3</f>
+        <f t="shared" ref="H3:H43" si="2">D3/E3</f>
         <v>0.67368421052631577</v>
       </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -5028,6 +6591,7 @@
         <f t="shared" si="2"/>
         <v>0.68085106382978722</v>
       </c>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -5057,6 +6621,7 @@
         <f t="shared" si="2"/>
         <v>0.65306122448979587</v>
       </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -5086,6 +6651,7 @@
         <f t="shared" si="2"/>
         <v>0.65306122448979587</v>
       </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -5115,6 +6681,7 @@
         <f t="shared" si="2"/>
         <v>0.68817204301075274</v>
       </c>
+      <c r="I7" s="1"/>
       <c r="M7" t="s">
         <v>0</v>
       </c>
@@ -5147,6 +6714,7 @@
         <f t="shared" si="2"/>
         <v>0.87671232876712324</v>
       </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -5176,6 +6744,7 @@
         <f t="shared" si="2"/>
         <v>0.7441860465116279</v>
       </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -5205,6 +6774,7 @@
         <f t="shared" si="2"/>
         <v>0.68817204301075274</v>
       </c>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -5234,6 +6804,7 @@
         <f t="shared" si="2"/>
         <v>0.7191011235955056</v>
       </c>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -5263,6 +6834,7 @@
         <f t="shared" si="2"/>
         <v>0.79012345679012341</v>
       </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -5292,6 +6864,7 @@
         <f t="shared" si="2"/>
         <v>0.82051282051282048</v>
       </c>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -5321,6 +6894,7 @@
         <f t="shared" si="2"/>
         <v>0.82051282051282048</v>
       </c>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -5350,6 +6924,7 @@
         <f t="shared" si="2"/>
         <v>0.91428571428571426</v>
       </c>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -5379,8 +6954,9 @@
         <f t="shared" si="2"/>
         <v>0.87671232876712324</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>527</v>
       </c>
@@ -5408,8 +6984,9 @@
         <f t="shared" si="2"/>
         <v>0.92753623188405798</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>528</v>
       </c>
@@ -5437,8 +7014,9 @@
         <f t="shared" si="2"/>
         <v>0.94117647058823528</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>531</v>
       </c>
@@ -5466,8 +7044,9 @@
         <f t="shared" si="2"/>
         <v>0.98461538461538467</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>538</v>
       </c>
@@ -5495,8 +7074,9 @@
         <f t="shared" si="2"/>
         <v>0.92753623188405798</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>526</v>
       </c>
@@ -5524,8 +7104,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>536</v>
       </c>
@@ -5553,8 +7134,9 @@
         <f t="shared" si="2"/>
         <v>0.95522388059701491</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>528</v>
       </c>
@@ -5582,8 +7164,9 @@
         <f t="shared" si="2"/>
         <v>0.95522388059701491</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>526</v>
       </c>
@@ -5611,8 +7194,9 @@
         <f t="shared" si="2"/>
         <v>0.98461538461538467</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>536</v>
       </c>
@@ -5640,8 +7224,9 @@
         <f t="shared" si="2"/>
         <v>0.96969696969696972</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>525</v>
       </c>
@@ -5669,8 +7254,9 @@
         <f t="shared" si="2"/>
         <v>0.98461538461538467</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>534</v>
       </c>
@@ -5698,8 +7284,9 @@
         <f t="shared" si="2"/>
         <v>0.98461538461538467</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>534</v>
       </c>
@@ -5727,8 +7314,9 @@
         <f t="shared" si="2"/>
         <v>1.0151515151515151</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>534</v>
       </c>
@@ -5756,8 +7344,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>532</v>
       </c>
@@ -5785,8 +7374,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>534</v>
       </c>
@@ -5814,8 +7404,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>534</v>
       </c>
@@ -5843,8 +7434,9 @@
         <f t="shared" si="2"/>
         <v>1.03125</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>531</v>
       </c>
@@ -5872,8 +7464,9 @@
         <f t="shared" si="2"/>
         <v>1.140625</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>532</v>
       </c>
@@ -5901,8 +7494,9 @@
         <f t="shared" si="2"/>
         <v>0.91549295774647887</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>532</v>
       </c>
@@ -5930,8 +7524,9 @@
         <f t="shared" si="2"/>
         <v>1.046875</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>527</v>
       </c>
@@ -5959,8 +7554,9 @@
         <f t="shared" si="2"/>
         <v>1.03125</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>532</v>
       </c>
@@ -5988,8 +7584,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>531</v>
       </c>
@@ -6017,8 +7614,9 @@
         <f t="shared" si="2"/>
         <v>1.1875</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>531</v>
       </c>
@@ -6046,8 +7644,9 @@
         <f t="shared" si="2"/>
         <v>1.046875</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>527</v>
       </c>
@@ -6075,8 +7674,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>527</v>
       </c>
@@ -6104,8 +7704,9 @@
         <f t="shared" si="2"/>
         <v>1.09375</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>530</v>
       </c>
@@ -6133,8 +7734,9 @@
         <f t="shared" si="2"/>
         <v>1.125</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>531</v>
       </c>
@@ -6162,6 +7764,7 @@
         <f t="shared" si="2"/>
         <v>0.98461538461538467</v>
       </c>
+      <c r="I43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More and more readings
</commit_message>
<xml_diff>
--- a/motor analysis.xlsx
+++ b/motor analysis.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>LPWM</t>
   </si>
 </sst>
 </file>
@@ -512,11 +515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="369991184"/>
-        <c:axId val="369990064"/>
+        <c:axId val="313951392"/>
+        <c:axId val="310660384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="369991184"/>
+        <c:axId val="313951392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +562,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369990064"/>
+        <c:crossAx val="310660384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -567,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="369990064"/>
+        <c:axId val="310660384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +621,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="369991184"/>
+        <c:crossAx val="313951392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,11 +1466,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="365884864"/>
-        <c:axId val="365891584"/>
+        <c:axId val="256433264"/>
+        <c:axId val="255370208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="365884864"/>
+        <c:axId val="256433264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,12 +1513,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365891584"/>
+        <c:crossAx val="255370208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="365891584"/>
+        <c:axId val="255370208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1569,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365884864"/>
+        <c:crossAx val="256433264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1629,20 +1632,539 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>left motor pwm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16534711286089238"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Left to Right ratio</c:v>
+            <c:strRef>
+              <c:f>Forward!$F$2:$F$43</c:f>
+              <c:strCache>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>80768,9375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77235,125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55540,875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47285,8125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42148,0625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34722,875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38767,6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36029,75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34862,75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35939,1875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34408,375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33812,0625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32287,25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31100,25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31473,4375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29832,125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27391,9375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28302,0625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581,5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26248,625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25835,5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24737,9375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23201,5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22625,5625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22460,875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19954,68657</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928,125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053,0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998,4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18668,66667</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17709,80822</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19098,83077</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18679,8806</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17931,93939</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826,75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15197,10526</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16984,89552</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348,4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15816,88889</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14941,8125</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Forward!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>80768.9375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77235.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55540.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47285.8125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42148.0625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34722.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38767.6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36029.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34862.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35939.1875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34408.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33812.0625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32287.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31100.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31473.4375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29832.125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27391.9375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28302.0625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26248.625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25835.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24737.9375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23201.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22625.5625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22460.875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19954.686567164179</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928.125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053.0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998.4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18668.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17709.808219178081</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19098.830769230768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18679.880597014926</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17931.939393939392</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15197.105263157895</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16984.895522388058</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348.4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15816.888888888889</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14941.8125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Forward!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Forward!$F$2:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>80768,9375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77235,125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55540,875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47285,8125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42148,0625</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1651,11 +2173,204 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:name>lm</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="0.00000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>Forward2!$B$2:$B$43</c:f>
+              <c:f>Forward!$F$2:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>80768.9375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77235.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55540.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47285.8125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42148.0625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34722.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38767.6875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36029.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34862.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35939.1875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34408.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33812.0625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32287.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31100.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31473.4375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29832.125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27391.9375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28302.0625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26248.625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25835.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24737.9375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23201.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22625.5625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22460.875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19954.686567164179</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928.125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053.0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998.4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18668.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17709.808219178081</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19098.830769230768</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18679.880597014926</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17931.939393939392</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15197.105263157895</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16984.895522388058</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348.4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15816.888888888889</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14941.8125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Forward!$B$2:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
@@ -1787,295 +2502,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Forward2!$H$2:$H$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
-                <c:pt idx="0">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86486486486486491</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.7441860465116279</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.68817204301075274</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.72727272727272729</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.79012345679012341</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.82051282051282048</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.84210526315789469</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.83116883116883122</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.810126582278481</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.92957746478873238</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.87671232876712324</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.84210526315789469</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.86486486486486491</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.95522388059701491</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.96969696969696972</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.92753623188405798</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.015625</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.09375</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.91428571428571426</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.046875</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.078125</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.0625</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.125</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.15625</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.21875</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.0625</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.015625</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.1875</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.09375</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.0625</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>fw1</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Forward!$H$2:$H$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>0.82051282051282048</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67368421052631577</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.68085106382978722</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.65306122448979587</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65306122448979587</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.68817204301075274</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.87671232876712324</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7441860465116279</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.68817204301075274</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.7191011235955056</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.79012345679012341</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.82051282051282048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.82051282051282048</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.91428571428571426</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.87671232876712324</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.92753623188405798</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.94117647058823528</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.92753623188405798</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.95522388059701491</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.95522388059701491</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.96969696969696972</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.98461538461538467</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.0151515151515151</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.140625</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.91549295774647887</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.046875</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.03125</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.1875</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.046875</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.09375</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2085,17 +2513,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="368413408"/>
-        <c:axId val="368410048"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="368413408"/>
+        <c:axId val="370581472"/>
+        <c:axId val="370582032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370581472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2105,8 +2546,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2133,15 +2574,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368410048"/>
+        <c:crossAx val="370582032"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="368410048"/>
+        <c:axId val="370582032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,8 +2605,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2192,9 +2636,9 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368413408"/>
+        <c:crossAx val="370581472"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2256,7 +2700,1265 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>right motor pwm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16534711286089238"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Forward!$G$2:$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>66271,94872</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52032,08421</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42487,14894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36271,59184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30880,53061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29005,11828</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>lm</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="0.00000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Forward!$G$2:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>66271.948717948719</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52032.084210526315</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42487.148936170212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36271.591836734697</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30880.530612244896</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29005.118279569891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30441.972602739726</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28850.372093023256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24794.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25069.842696629214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28396.395061728395</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28232.51282051282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27743.23076923077</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29519.771428571428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27265.972602739726</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29192.753623188404</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28077.294117647059</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26970.523076923077</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26251.1884057971</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26581.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25073.313432835821</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24678.686567164179</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24357.353846153845</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22498.424242424244</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22277.476923076923</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22115.323076923076</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20257.030303030304</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21928.125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>21053.0625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20998.4375</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19252.0625</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20200.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17484.845070422536</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19555.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18492.3125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>18826.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18046.5625</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17781.0625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17348.4375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17983.4375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17794</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14711.938461538462</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Forward!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370584832"/>
+        <c:axId val="370585392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370584832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370585392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="370585392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370584832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Left to Right ratio</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Forward2!$B$2:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Forward2!$H$2:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="42"/>
+                <c:pt idx="0">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86486486486486491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7441860465116279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68817204301075274</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79012345679012341</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82051282051282048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84210526315789469</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83116883116883122</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.810126582278481</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.92957746478873238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.87671232876712324</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.84210526315789469</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.86486486486486491</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95522388059701491</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92753623188405798</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.015625</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.09375</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.046875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.078125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.15625</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.21875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.015625</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.09375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>fw1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Forward!$H$2:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.82051282051282048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67368421052631577</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68085106382978722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65306122448979587</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65306122448979587</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68817204301075274</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.87671232876712324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7441860465116279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68817204301075274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7191011235955056</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79012345679012341</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82051282051282048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82051282051282048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87671232876712324</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.92753623188405798</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92753623188405798</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.95522388059701491</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95522388059701491</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0151515151515151</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.140625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.91549295774647887</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.046875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.03125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.046875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.09375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="370724416"/>
+        <c:axId val="370724976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="370724416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370724976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="370724976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370724416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2591,11 +4293,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="399683200"/>
-        <c:axId val="399690480"/>
+        <c:axId val="370727216"/>
+        <c:axId val="370727776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="399683200"/>
+        <c:axId val="370727216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +4340,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399690480"/>
+        <c:crossAx val="370727776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2646,7 +4348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399690480"/>
+        <c:axId val="370727776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,7 +4399,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399683200"/>
+        <c:crossAx val="370727216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2746,7 +4448,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2761,7 +4463,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3090,11 +4791,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="384375728"/>
-        <c:axId val="384376288"/>
+        <c:axId val="370730016"/>
+        <c:axId val="370730576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="384375728"/>
+        <c:axId val="370730016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,7 +4838,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384376288"/>
+        <c:crossAx val="370730576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3145,7 +4846,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="384376288"/>
+        <c:axId val="370730576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3196,7 +4897,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384375728"/>
+        <c:crossAx val="370730016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3445,6 +5146,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4478,7 +6259,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4505,8 +6286,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4586,11 +6367,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4601,11 +6377,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4617,7 +6388,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4637,9 +6408,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4652,10 +6420,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4695,22 +6463,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4815,8 +6584,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4948,19 +6717,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4974,6 +6744,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4994,7 +6775,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5021,8 +6802,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5102,6 +6883,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
@@ -5509,7 +7806,523 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6060,15 +8873,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>704849</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6082,6 +8895,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6466,8 +9341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6532,6 +9407,13 @@
         <v>0.82051282051282048</v>
       </c>
       <c r="I2" s="1"/>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="e">
+        <f>6892550.92794713 * POWER(K2, -1.05923146)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -6550,11 +9432,11 @@
         <v>95</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F44" si="0">C3/D3</f>
+        <f t="shared" ref="F3:F43" si="0">C3/D3</f>
         <v>77235.125</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G44" si="1">C3/E3</f>
+        <f t="shared" ref="G3:G43" si="1">C3/E3</f>
         <v>52032.084210526315</v>
       </c>
       <c r="H3">
@@ -7846,15 +10728,15 @@
         <v>74</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F44" si="0">C3/D3</f>
+        <f t="shared" ref="F3:F43" si="0">C3/D3</f>
         <v>69595.875</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G44" si="1">C3/E3</f>
+        <f t="shared" ref="G3:G43" si="1">C3/E3</f>
         <v>60191.027027027027</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H44" si="2">D3/E3</f>
+        <f t="shared" ref="H3:H43" si="2">D3/E3</f>
         <v>0.86486486486486491</v>
       </c>
     </row>

</xml_diff>